<commit_message>
Parse all and save excel
</commit_message>
<xml_diff>
--- a/usmoll.xlsx
+++ b/usmoll.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="263">
   <si>
     <t>Каталог</t>
   </si>
@@ -46,10 +46,10 @@
     <t>Цена</t>
   </si>
   <si>
-    <t>Описание товара</t>
-  </si>
-  <si>
-    <t>Ссылки на картинки</t>
+    <t>Описание товара Rus</t>
+  </si>
+  <si>
+    <t>Описание товара Eng</t>
   </si>
   <si>
     <t>Цвета</t>
@@ -58,142 +58,179 @@
     <t>Размеры</t>
   </si>
   <si>
-    <t>Мальчики</t>
-  </si>
-  <si>
-    <t>Одежда</t>
-  </si>
-  <si>
-    <t>Пижамы</t>
+    <t/>
+  </si>
+  <si>
+    <t>Уютный халат с длинными рукавами для мальчиков Big Boy</t>
+  </si>
+  <si>
+    <t>Big Boys Long Sleeve Cozy Robe</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4810502-big-boys-long-sleeve-cozy-robe-calvin-klein</t>
+  </si>
+  <si>
+    <t>4810502</t>
   </si>
   <si>
     <t>Calvin Klein</t>
   </si>
   <si>
-    <t>Big Boys Long Sleeve Cozy Robe</t>
-  </si>
-  <si>
-    <t>Уютный халат с длинными рукавами для мальчиков Big Boy Calvin Klein</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4810502-big-boys-long-sleeve-cozy-robe-calvin-klein</t>
-  </si>
-  <si>
-    <t>4810502</t>
-  </si>
-  <si>
-    <t>Ремень для галстукаБез капюшонаКарманыЭтот предмет, приобретенный через Интернет, должен быть возвращен продавцу только по почте. Этот предмет нельзя вернуть в магазины Macy's.100% полиэстер Джерси с классом огнестойкостиМожно стирать в машине</t>
+    <t>Уютный халат с вышитым логотипом Calvin Klein, завязывающимся поясом и двумя карманами для максимального комфорта.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Ремень для галстука&lt;/li&gt;&lt;li&gt;Без капюшона&lt;/li&gt;&lt;li&gt;Карманы&lt;/li&gt;&lt;li&gt;Этот предмет, приобретенный через Интернет, должен быть возвращен продавцу только по почте. Этот предмет нельзя вернуть в магазины Macy's.&lt;/li&gt;&lt;li&gt;100% полиэстер Джерси с классом огнестойкости&lt;/li&gt;&lt;li&gt;Можно стирать в машине&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Calvin Klein embroidered logo cozy robe with tie belt and two pockets for the ultimate comfort.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Tie belt&lt;/li&gt;&lt;li&gt;No hood&lt;/li&gt;&lt;li&gt;Pockets&lt;/li&gt;&lt;li&gt;100% Fire Resistance Rating Polyester Jersey&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[серый]</t>
+  </si>
+  <si>
+    <t>[S M L XL]</t>
+  </si>
+  <si>
+    <t>серый</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/481/05/02/625737335b67d8d54d3ea5362bbf7334.jpeg https://usmall.ru/image/481/05/02/49a9c7cf1dac75e7954c43b92cc7ae97.jpeg https://usmall.ru/image/481/05/02/47bb97c51fc253803cb58d62ab8b25f6.jpeg]</t>
   </si>
   <si>
-    <t>[Серый (Slate Gray Camo)]</t>
-  </si>
-  <si>
-    <t>[S M L XL]</t>
-  </si>
-  <si>
-    <t>Событие</t>
-  </si>
-  <si>
-    <t>На выход</t>
-  </si>
-  <si>
-    <t>Способ ухода</t>
-  </si>
-  <si>
-    <t>Машинная стирка</t>
-  </si>
-  <si>
-    <t>Длина рукава</t>
-  </si>
-  <si>
-    <t>Длинные</t>
+    <t>Baby Boys and Girls Plush Bathrobe and Toy, 2-Piece Set</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4862430-baby-boys-and-girls-plush-bathrobe-and-toy-2-piece-set-hudson-baby</t>
+  </si>
+  <si>
+    <t>4862430</t>
   </si>
   <si>
     <t>Hudson Baby</t>
   </si>
   <si>
-    <t>Baby Boys and Girls Plush Bathrobe and Toy, 2-Piece Set</t>
-  </si>
-  <si>
-    <t>Baby Boys and Girls Plush Bathrobe and Toy, 2-Piece Set Hudson Baby</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4862430-baby-boys-and-girls-plush-bathrobe-and-toy-2-piece-set-hudson-baby</t>
-  </si>
-  <si>
-    <t>4862430</t>
-  </si>
-  <si>
-    <t>Set includes - 1 plush bathrobe and 1 toySoft and gentle on baby's skinPerfect baby shower giftThis item purchased online must be returned to the vendor by mail only. This item cannot be returned to Macy's stores.100% PolyesterMachine Washable</t>
+    <t>Hudson Baby plush robe and toy set is a great gift set for baby. Our super soft bathrobe and matching plush toy is perfect for snuggling up and getting cozy for bed at the end of a long day.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Set includes - 1 plush bathrobe and 1 toy&lt;/li&gt;&lt;li&gt;Soft and gentle on baby's skin&lt;/li&gt;&lt;li&gt;Perfect baby shower gift&lt;/li&gt;&lt;li&gt;This item purchased online must be returned to the vendor by mail only. This item cannot be returned to Macy's stores.&lt;/li&gt;&lt;li&gt;100% Polyester&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[желтый]</t>
+  </si>
+  <si>
+    <t>[One Size Fits All]</t>
+  </si>
+  <si>
+    <t>желтый</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/486/24/30/37823e18d9ccfb63bfe71079cdfb046d.jpeg https://usmall.ru/image/486/24/30/d69c90cccfffe5332944ddd567debe57.jpeg https://usmall.ru/image/486/24/30/11acef3aeb3fcd665d9bd3a734ba7be4.jpeg]</t>
   </si>
   <si>
-    <t>[Желтый (Yellow Duck)]</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>Фасон</t>
-  </si>
-  <si>
-    <t>Пижамные</t>
-  </si>
-  <si>
-    <t>Халаты</t>
+    <t>Халат без капюшона (для больших детей)</t>
+  </si>
+  <si>
+    <t>Non Hooded Robe (Big Kids)</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/5056636-non-hooded-robe-big-kids-hurley-kids</t>
+  </si>
+  <si>
+    <t>5056636</t>
+  </si>
+  <si>
+    <t>Hurley Kids</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Проведите веселый день у бассейна, отдыхая в непринужденном халате без капюшона Hurley® Kids.&lt;/li&gt;
+&lt;li&gt;Дизайн клетчатого узора.&lt;/li&gt;
+&lt;li&gt;Открытый фронт.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Шаль воротник.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Длинные рукава с широкой резинкой.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Брендинг на левой груди.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Самостоятельная завязка на талии шлевками для ремня.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Модель прямого силуэта.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;100% полиэстер.&lt;/li&gt;
+&lt;li&gt;Машинная стирка, сушка в стиральной машине.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;li&gt;Размеры:&lt;ul&gt;&lt;li&gt;Длина: 38 дюймов&lt;/li&gt;
+    &lt;li&gt;Длина рукава: 30 дюймов&lt;/li&gt;
+    &lt;/ul&gt;&lt;/li&gt;
+&lt;li&gt;Измерения продукта проводились с использованием размера XL (18/20 Big Kid). Заметьте, пожалуйста, что измерения могут быть разной величины.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Have a fun day around the pool lounging in the super relaxed Hurley® Kids Non Hooded Robe.&lt;/li&gt;
+&lt;li&gt;Plaid pattern design.&lt;/li&gt;
+&lt;li&gt;Open front.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Shawl collar.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Long sleeves with banded cuffs.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Branding on left chest.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Self-tie at the waist with belt loops.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Straight hemline.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;100% polyester.&lt;/li&gt;
+&lt;li&gt; Machine wash, tumble dry.&lt;br /&gt;&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;li&gt;Measurements:
+&lt;ul&gt;&lt;li&gt; Length: 38 in&lt;/li&gt;
+    &lt;li&gt; Sleeve Length: 30 in&lt;/li&gt;
+    &lt;/ul&gt;&lt;/li&gt;
+&lt;li&gt;Product measurements were taken using size XL (18/20 Big Kid). Please note that measurements may vary by size.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[красный]</t>
+  </si>
+  <si>
+    <t>[SM (8 Big Kid) One Size MD (10/12 Big Kid) One Size LG (14/16 Big Kid) One Size XL (18/20 Big Kid) One Size]</t>
+  </si>
+  <si>
+    <t>красный</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/505/66/36/2a94c535486303e24a53ccc70b080cde.jpeg]</t>
+  </si>
+  <si>
+    <t>Набор из халата и тапочек Lego Star Wars для мальчиков 4–12 лет для мальчиков 4–12 лет</t>
+  </si>
+  <si>
+    <t>Boys 4-12 Lego Star Wars Boys Robe &amp; Slippers Set</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/3439266-boys-4-12-lego-star-wars-boys-robe-slippers-set-licensed-character</t>
+  </si>
+  <si>
+    <t>3439266</t>
   </si>
   <si>
     <t>Licensed Character</t>
   </si>
   <si>
-    <t>Boys 4-12 Lego Star Wars Boys Robe &amp; Slippers Set</t>
-  </si>
-  <si>
-    <t>Набор из халата и тапочек Lego Star Wars для мальчиков 4–12 лет для мальчиков 4–12 лет Licensed Character</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/3439266-boys-4-12-lego-star-wars-boys-robe-slippers-set-licensed-character</t>
-  </si>
-  <si>
-    <t>3439266</t>
-  </si>
-  <si>
-    <t>Полиэстер В целях безопасности детей одежда должна быть плотно прилегающей или огнестойкой. Это огнестойкая одежда. Машинная стирка Импортные</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/343/92/66/0ab94bbeb5e6782aaa8ccbcc993efea4.jpeg https://usmall.ruhttps://app.usmall.ru/image/39758543 https://usmall.ru/image/000/00/00/40a658070482bd804220beabf888ef0f.jpeg https://usmall.ru/image/000/00/00/26923d95d420c51d685b538a05f16842.jpeg https://usmall.ru/image/000/00/00/4b08bab15d7564e2b1e23380c265b001.jpeg]</t>
-  </si>
-  <si>
-    <t>[Красный (Red)]</t>
+    <t>&lt;p&gt;Ему понравится готовиться ко сну с этим набором халата и тапочек для мальчиков Lego Star Wars.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;В наборе 2 предмета: халат и тапочки.&lt;/li&gt; &lt;li&gt;Верх: круглый вырез, длинные рукава&lt;/li&gt; &lt;li&gt;Низ: эластичный пояс&lt;/li&gt; &lt;li&gt;Халат размера 4/5 = тапочки размера 9/10, халат размера 6/7 = тапочки размера 11/12, халат размера 8/9 = тапочки размера 13/1, халат размера 10/12 = тапочки размера 2/3&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ТКАНИ И УХОД&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Полиэстер&lt;/li&gt; &lt;li&gt;В целях безопасности детей одежда должна быть плотно прилегающей или огнестойкой. Это огнестойкая одежда.&lt;/li&gt; &lt;li&gt;Машинная стирка&lt;/li&gt; &lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; He'll love getting ready for bed with this boys' Lego Star Wars Boys Robe and Slippers Set. &lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;2-piece set includes: robe &amp;amp; slippers&lt;/li&gt; &lt;li&gt;Top: crewneck, long sleeves&lt;/li&gt; &lt;li&gt;Bottoms: elastic waistband&lt;/li&gt; &lt;li&gt;Size 4/5 robe = size 9/10 slipper, size 6/7 robe = size 11/12 slipper, size 8/9 robe = size 13/1 slipper, size 10/12 robe = size 2/3 slipper&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;FABRIC &amp;amp; CARE&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polyester&lt;/li&gt; &lt;li&gt;For children's safety, garments should be snug fitting or flame resistant. These are flame resistant garments.&lt;/li&gt; &lt;li&gt;Machine wash&lt;/li&gt; &lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[4-5]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/343/92/66/0ab94bbeb5e6782aaa8ccbcc993efea4.jpeg https://app.usmall.ru/image/39758543 https://usmall.ru/image/000/00/00/40a658070482bd804220beabf888ef0f.jpeg https://usmall.ru/image/000/00/00/26923d95d420c51d685b538a05f16842.jpeg https://usmall.ru/image/000/00/00/4b08bab15d7564e2b1e23380c265b001.jpeg]</t>
+  </si>
+  <si>
+    <t>Toddler|Child Boys Fleece Sleep Robe - Soft &amp; Cozy Kids Bathrobe</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/5081179-toddlerchild-boys-fleece-sleep-robe-soft-cozy-kids-bathrobe-jellifish-kids</t>
+  </si>
+  <si>
+    <t>5081179</t>
   </si>
   <si>
     <t>Jellifish Kids</t>
   </si>
   <si>
-    <t>Toddler|Child Boys Fleece Sleep Robe - Soft &amp; Cozy Kids Bathrobe</t>
-  </si>
-  <si>
-    <t>Toddler|Child Boys Fleece Sleep Robe - Soft &amp; Cozy Kids Bathrobe Jellifish Kids</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/5081179-toddlerchild-boys-fleece-sleep-robe-soft-cozy-kids-bathrobe-jellifish-kids</t>
-  </si>
-  <si>
-    <t>5081179</t>
-  </si>
-  <si>
-    <t>Soft 100% polyester flannel fleece fabric3D animal ear hoodTie-belt at the waist for the perfect fitLong sleeves for added warmthDeep pockets perfect for anything you need to carry with you100% Polyester Flannel Fleece (200 Gsm)Machine washable</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/508/11/79/7a24ed87bd90a6acf19db40f4a054bc2.jpeg https://usmall.ruhttps://app.usmall.ru/image/42136590 https://usmall.ruhttps://app.usmall.ru/image/42136591]</t>
-  </si>
-  <si>
-    <t>[Красный (Red Bear)]</t>
+    <t>These soft, plush sleep robes are perfect for getting out of the bath or for chilly nights. Made from 100% Polyester Flannel Fleece, these robes are durable and will not be worn out by your little one. Available in pink and purple, they come with deep pockets and hood for added functionality.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Soft 100% polyester flannel fleece fabric&lt;/li&gt;&lt;li&gt;3D animal ear hood&lt;/li&gt;&lt;li&gt;Tie-belt at the waist for the perfect fit&lt;/li&gt;&lt;li&gt;Long sleeves for added warmth&lt;/li&gt;&lt;li&gt;Deep pockets perfect for anything you need to carry with you&lt;/li&gt;&lt;li&gt;100% Polyester Flannel Fleece (200 Gsm)&lt;/li&gt;&lt;li&gt;Machine washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[XSmall Small Medium Large XLarge]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/508/11/79/7a24ed87bd90a6acf19db40f4a054bc2.jpeg https://app.usmall.ru/image/42136590 https://app.usmall.ru/image/42136591]</t>
   </si>
   <si>
     <t>https://usmall.ru/product/5075601-toddlerchild-boys-fleece-sleep-robe-soft-cozy-kids-bathrobe-jellifish-kids</t>
@@ -202,269 +239,279 @@
     <t>5075601</t>
   </si>
   <si>
-    <t>Soft 100% polyester flannel fleece fabric3D animal ear hoodTie-belt at the waist for the perfect fitLong sleeves for added warmthDeep pockets perfect for anything you need to carry with you100% Polyester Frosted Plush (200 Gsm)Machine washable</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/507/56/01/cc906bace099624eb660ec24a0a49354.jpeg https://usmall.ruhttps://app.usmall.ru/image/42084203 https://usmall.ruhttps://app.usmall.ru/image/42084204]</t>
-  </si>
-  <si>
-    <t>[Серый (Grey Plush) Синий (Navy Plush)]</t>
-  </si>
-  <si>
-    <t>Hurley Kids</t>
-  </si>
-  <si>
-    <t>Non Hooded Robe (Big Kids)</t>
-  </si>
-  <si>
-    <t>Халат без капюшона (для больших детей) Hurley Kids</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/5056636-non-hooded-robe-big-kids-hurley-kids</t>
-  </si>
-  <si>
-    <t>5056636</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Длина: 38 дюймов
-Длина рукава: 30 дюймов
-</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/505/66/36/2a94c535486303e24a53ccc70b080cde.jpeg]</t>
-  </si>
-  <si>
-    <t>[Красный (Gym Red)]</t>
-  </si>
-  <si>
-    <t>Материал</t>
-  </si>
-  <si>
-    <t>Полиэстер</t>
-  </si>
-  <si>
-    <t>Узор</t>
-  </si>
-  <si>
-    <t>Клетка</t>
+    <t>These soft, plush sleep robes are perfect for getting out of the bath or for chilly nights. Made from 100% Polyester Flannel Fleece, these robes are durable and will not be worn out by your little one. Available in pink and purple, they come with deep pockets and hood for added functionality.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Soft 100% polyester flannel fleece fabric&lt;/li&gt;&lt;li&gt;3D animal ear hood&lt;/li&gt;&lt;li&gt;Tie-belt at the waist for the perfect fit&lt;/li&gt;&lt;li&gt;Long sleeves for added warmth&lt;/li&gt;&lt;li&gt;Deep pockets perfect for anything you need to carry with you&lt;/li&gt;&lt;li&gt;100% Polyester Frosted Plush (200 Gsm)&lt;/li&gt;&lt;li&gt;Machine washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[серый синий]</t>
+  </si>
+  <si>
+    <t>[XSmall Small Medium]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/507/56/01/cc906bace099624eb660ec24a0a49354.jpeg https://app.usmall.ru/image/42084203 https://app.usmall.ru/image/42084204]</t>
+  </si>
+  <si>
+    <t>синий</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/42084198 https://app.usmall.ru/image/42084199 https://app.usmall.ru/image/42084200]</t>
+  </si>
+  <si>
+    <t>Sleep On It Boys Yeti Monster Plush Fleece Robe with 3D Character Hood</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/5027669-sleep-on-it-boys-yeti-monster-plush-fleece-robe-with-3d-character-hood-sleep-on-it</t>
+  </si>
+  <si>
+    <t>5027669</t>
   </si>
   <si>
     <t>Sleep On It</t>
   </si>
   <si>
-    <t>Sleep On It Boys Yeti Monster Plush Fleece Robe with 3D Character Hood</t>
-  </si>
-  <si>
-    <t>Sleep On It Boys Yeti Monster Plush Fleece Robe with 3D Character Hood Sleep On It</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/5027669-sleep-on-it-boys-yeti-monster-plush-fleece-robe-with-3d-character-hood-sleep-on-it</t>
-  </si>
-  <si>
-    <t>5027669</t>
-  </si>
-  <si>
-    <t>Hooded Robe with Front Tie100% Plush Flannel FleeceBuilt Up 3D Charachter HoodMeant to be Loose FittingFlame resistantPolyesterMachine WashImported</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/502/76/69/f878d7faf8a2d915d794066c725f0664.jpeg https://usmall.ruhttps://app.usmall.ru/image/41584770 https://usmall.ruhttps://app.usmall.ru/image/41584769]</t>
-  </si>
-  <si>
-    <t>[Синий (Blue)]</t>
+    <t>&lt;p&gt;He loves hanging out in the forest and staying up late, and we hear he can be lured out of hiding with peanut butter and goldfish crackers. Is it the mythical sasquatch, or just the cutest little boy getting ready for bed? You'll never know for sure when he's donning this novelty robe made with warm and cozy flannel fleece.&lt;/p&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Hooded Robe with Front Tie&lt;/li&gt;&lt;li&gt;100% Plush Flannel Fleece&lt;/li&gt;&lt;li&gt;Built Up 3D Charachter Hood&lt;/li&gt;&lt;li&gt;Meant to be Loose Fitting&lt;/li&gt;&lt;li&gt;Flame resistant&lt;/li&gt;&lt;li&gt;Polyester&lt;/li&gt;&lt;li&gt;Machine Wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[синий]</t>
+  </si>
+  <si>
+    <t>[MEDIUM]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/502/76/69/f878d7faf8a2d915d794066c725f0664.jpeg https://app.usmall.ru/image/41584770 https://app.usmall.ru/image/41584769]</t>
+  </si>
+  <si>
+    <t>Халат с длинными рукавами и тапочки для маленьких мальчиков, комплект из 2 предметов</t>
+  </si>
+  <si>
+    <t>Little Boys Long Sleeve Robe with Slippers, 2 Piece Set</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4885607-little-boys-long-sleeve-robe-with-slippers-2-piece-set-max-olivia</t>
+  </si>
+  <si>
+    <t>4885607</t>
   </si>
   <si>
     <t>Max &amp; Olivia</t>
   </si>
   <si>
-    <t>Little Boys Long Sleeve Robe with Slippers, 2 Piece Set</t>
-  </si>
-  <si>
-    <t>Халат с длинными рукавами и тапочки для маленьких мальчиков, комплект из 2 предметов Max &amp; Olivia</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4885607-little-boys-long-sleeve-robe-with-slippers-2-piece-set-max-olivia</t>
-  </si>
-  <si>
-    <t>4885607</t>
-  </si>
-  <si>
-    <t>В комплект входит- 1 халат и 1 пара тапочек.Длинный рукавХалат с поясом и шалевым воротникомЭтот предмет, приобретенный через Интернет, должен быть возвращен продавцу только по почте. Этот предмет нельзя вернуть в магазины Macy's.100% полиэстерМожно стирать в машине</t>
+    <t>Согрейтесь, отдыхая в этом уютном плюшевом халате из флиса с подходящими тапочками.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;В комплект входит- 1 халат и 1 пара тапочек.&lt;/li&gt;&lt;li&gt;Длинный рукав&lt;/li&gt;&lt;li&gt;Халат с поясом и шалевым воротником&lt;/li&gt;&lt;li&gt;Этот предмет, приобретенный через Интернет, должен быть возвращен продавцу только по почте. Этот предмет нельзя вернуть в магазины Macy's.&lt;/li&gt;&lt;li&gt;100% полиэстер&lt;/li&gt;&lt;li&gt;Можно стирать в машине&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Keep warm lounging in this cozy, plush fleece robe with matching slippers.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Set includes- 1 robe and 1 pair of slippers&lt;/li&gt;&lt;li&gt;Long sleeve&lt;/li&gt;&lt;li&gt;Belted robe with shawl collar&lt;/li&gt;&lt;li&gt;This item purchased online must be returned to the vendor by mail only. This item cannot be returned to Macy's stores.&lt;/li&gt;&lt;li&gt;100% Polyester&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[S (6/7)]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/471/44/76/1cf79519c53317b385405c2f55476557.jpeg]</t>
   </si>
   <si>
-    <t>[Синий (Navy)]</t>
+    <t>Детский флисовый халат с капюшоном Leveret, оранжевый, 16 лет</t>
+  </si>
+  <si>
+    <t>Leveret Kids Fleece Hooded Robe Classic Solid Color</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4870695-leveret-kids-fleece-hooded-robe-classic-solid-color-leveret</t>
+  </si>
+  <si>
+    <t>4870695</t>
   </si>
   <si>
     <t>Leveret</t>
   </si>
   <si>
-    <t>Leveret Kids Fleece Hooded Robe Classic Solid Color</t>
-  </si>
-  <si>
-    <t>Детский флисовый халат с капюшоном Leveret, оранжевый, 16 лет Leveret</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4870695-leveret-kids-fleece-hooded-robe-classic-solid-color-leveret</t>
-  </si>
-  <si>
-    <t>4870695</t>
-  </si>
-  <si>
-    <t>100% полиэстер огнестойкий флисОтлично подходит для ношения поверх легкой пижамы в холодные ночи.Халат с капюшоном и завязывающимся поясом на талииМашинная стирка в холодной воде наизнанку100% полиэстерМашинная стиркаИмпортные</t>
+    <t>&lt;p&gt;Устройтесь поудобнее после холодного душа в детском халате с капюшоном из флиса! Они идеально подходят для ношения поверх других пижам, чтобы оставаться в тепле зимними ночами. Каждый продукт оснащен удобными карманами спереди, а также самозавязывающимся ремнем на талии для регулируемой посадки. Он также включает в себя стильный капюшон, чтобы завершить удобный вид, и есть много вариантов, чтобы сочетаться с остальными членами семьи. Цвета включают черный, пурпурный и другие цвета, чтобы ваш ребенок выглядел идеально. Размеры варьируются от 2 до 16 лет, имейте в виду, что изделия могут дать усадку после стирки. Детский флисовый халат с капюшоном обязательно станет удобным фаворитом! Лучший праздничный подарок на Рождество, Хануку или любой праздник или особый случай.&lt;/p&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;100% полиэстер огнестойкий флис&lt;/li&gt;&lt;li&gt;Отлично подходит для ношения поверх легкой пижамы в холодные ночи.&lt;/li&gt;&lt;li&gt;Халат с капюшоном и завязывающимся поясом на талии&lt;/li&gt;&lt;li&gt;Машинная стирка в холодной воде наизнанку&lt;/li&gt;&lt;li&gt;100% полиэстер&lt;/li&gt;&lt;li&gt;Машинная стирка&lt;/li&gt;&lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Get cozy after those cold showers with the Kids Fleece Hooded Robe! These are perfect for wearing on top of other pajamas to stay extra warm during the winter nights. Each product comes with convenient pockets at the front along with a self-tying belt at the waist for that adjustable fit. It also includes a stylish hood to complete the comfy look, and there are many options for matching with the rest of the family. Colors consist of black, magenta, plus others to get that perfect look for your child. Sizes range from ages 2 to 16 years old, keep in mind products may shrink after washing. The Kids Fleece Hooded Robe is bound to be a comfortable favorite! Best Holiday gift for Christmas, Hanukkah or any Holiday or special occasion.&lt;/p&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;100% Polyester Flame Resistant fleece&lt;/li&gt;&lt;li&gt;Great for wearing on top of lighter pj's on cold nights&lt;/li&gt;&lt;li&gt;Hooded robe featuring self-tie belt at waist&lt;/li&gt;&lt;li&gt;Machine Wash Cold, Inside Out&lt;/li&gt;&lt;li&gt;100% Polyester&lt;/li&gt;&lt;li&gt;Machine Wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[зеленый синий красный оранжевый желтый Пурпурный розовый]</t>
+  </si>
+  <si>
+    <t>[5T 16 10 12 3T 14 2T 8 4T 6]</t>
+  </si>
+  <si>
+    <t>Пурпурный</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/41584447]</t>
+  </si>
+  <si>
+    <t>розовый</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/43291117]</t>
+  </si>
+  <si>
+    <t>зеленый</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/487/06/95/d884f189a041e94cd355df57fe8591e1.jpeg]</t>
   </si>
   <si>
-    <t>[Розовый (Hot Pink) Красный (Red) Оранжевый (Orange) Желтый (Yellow) Зеленый (Green) Синий (Royal Blue) Пурпурный (Purple)]</t>
-  </si>
-  <si>
-    <t>[6 8 10 12 14 16 2T 3T 4T 5T]</t>
+    <t>[https://app.usmall.ru/image/41584449]</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/40491481]</t>
+  </si>
+  <si>
+    <t>оранжевый</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/39970143]</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/39970145]</t>
+  </si>
+  <si>
+    <t>Boy&amp;#8217;s Camo Robe</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4840902-boy8217s-camo-robe-petit-lem</t>
+  </si>
+  <si>
+    <t>4840902</t>
   </si>
   <si>
     <t>Petit Lem</t>
   </si>
   <si>
-    <t>Boy’s Camo Robe</t>
-  </si>
-  <si>
-    <t>Boy&amp;#8217;s Camo Robe Petit Lem</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4840902-boy8217s-camo-robe-petit-lem</t>
-  </si>
-  <si>
-    <t>4840902</t>
-  </si>
-  <si>
-    <t>Attached hoodLong sleevesOpen frontRemovable sashTwo front slip pocketsPolyesterMachine washImported</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/484/09/02/1c73dfb2a51a911b513282b80e996119.jpeg https://usmall.ruhttps://app.usmall.ru/image/39652546]</t>
-  </si>
-  <si>
-    <t>[Синий (BLUE)]</t>
-  </si>
-  <si>
-    <t>[8 12 14]</t>
+    <t>He’ll look cool in camouflage when it’s time for bed! Made with super plush fabric, this Petit Lem robe features a hood and a self-tie sash at the waist.&lt;ul&gt;&lt;li&gt;Attached hood&lt;/li&gt;&lt;li&gt;Long sleeves&lt;/li&gt;&lt;li&gt;Open front&lt;/li&gt;&lt;li&gt;Removable sash&lt;/li&gt;&lt;li&gt;Two front slip pockets&lt;/li&gt;&lt;li&gt;Polyester&lt;/li&gt;&lt;li&gt;Machine wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[12 14 8]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/484/09/02/1c73dfb2a51a911b513282b80e996119.jpeg https://app.usmall.ru/image/39652546]</t>
   </si>
   <si>
     <t>Boy's Game Controller Knit Hooded Robe</t>
   </si>
   <si>
-    <t>Boy's Game Controller Knit Hooded Robe Petit Lem</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4840867-boys-game-controller-knit-hooded-robe-petit-lem</t>
   </si>
   <si>
     <t>4840867</t>
   </si>
   <si>
-    <t>Attached hoodLong sleevesOpen frontSide slip pocketsDetachable beltPolyesterMachine washImported</t>
+    <t>This robe is knitted with a video game controller design and a hooded neckline.&lt;ul&gt;&lt;li&gt;Attached hood&lt;/li&gt;&lt;li&gt;Long sleeves&lt;/li&gt;&lt;li&gt;Open front&lt;/li&gt;&lt;li&gt;Side slip pockets&lt;/li&gt;&lt;li&gt;Detachable belt&lt;/li&gt;&lt;li&gt;Polyester&lt;/li&gt;&lt;li&gt;Machine wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[черный]</t>
+  </si>
+  <si>
+    <t>[14 8]</t>
+  </si>
+  <si>
+    <t>черный</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/484/08/67/6626d5e4dc704f46f73df6a0c83429e3.jpeg https://usmall.ru/image/484/08/67/6949c4a34c0223eb901e103afb721e24.jpeg]</t>
   </si>
   <si>
-    <t>[Черный (BLACK)]</t>
-  </si>
-  <si>
-    <t>[8 14]</t>
-  </si>
-  <si>
     <t>Little Boy's Patterned Hooded Robe</t>
   </si>
   <si>
-    <t>Little Boy's Patterned Hooded Robe Petit Lem</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4840854-little-boys-patterned-hooded-robe-petit-lem</t>
   </si>
   <si>
     <t>4840854</t>
   </si>
   <si>
+    <t>A comfortable patterned robe styled with an attached hood and a self-tie belt.&lt;ul&gt;&lt;li&gt;Attached hood&lt;/li&gt;&lt;li&gt;Long sleeves&lt;/li&gt;&lt;li&gt;Open front&lt;/li&gt;&lt;li&gt;Side slip pockets&lt;/li&gt;&lt;li&gt;Detachable belt&lt;/li&gt;&lt;li&gt;Polyester&lt;/li&gt;&lt;li&gt;Machine wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[2 3 4 5 6 7]</t>
+  </si>
+  <si>
     <t>[https://usmall.ru/image/484/08/54/05dc914cae05dfeee997bf4407d41669.jpeg https://usmall.ru/image/484/08/54/a838d964b3dd81e9ba923882a2550144.jpeg]</t>
   </si>
   <si>
-    <t>[Красный (BURGUNDY_MULTI)]</t>
-  </si>
-  <si>
-    <t>[2 3 4 5 6 7]</t>
-  </si>
-  <si>
     <t>Little Boy's Camouflage Fuzzy Hooded Robe</t>
   </si>
   <si>
-    <t>Little Boy's Camouflage Fuzzy Hooded Robe Petit Lem</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4826749-little-boys-camouflage-fuzzy-hooded-robe-petit-lem</t>
   </si>
   <si>
     <t>4826749</t>
   </si>
   <si>
-    <t>Attached hoodLong sleevesOpen frontTwo pocketsDetachable beltPolyesterMachine washImported</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/482/67/49/524fff8df06acbfe2d55650f97ff6616.jpeg https://usmall.ruhttps://app.usmall.ru/image/39508152]</t>
-  </si>
-  <si>
-    <t>[Зеленый (TEAL)]</t>
+    <t>This fuzzy robe in camouflage print has an attached hood and detachable belt.&lt;ul&gt;&lt;li&gt;Attached hood&lt;/li&gt;&lt;li&gt;Long sleeves&lt;/li&gt;&lt;li&gt;Open front&lt;/li&gt;&lt;li&gt;Two pockets&lt;/li&gt;&lt;li&gt;Detachable belt&lt;/li&gt;&lt;li&gt;Polyester&lt;/li&gt;&lt;li&gt;Machine wash&lt;/li&gt;&lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[зеленый]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/482/67/49/524fff8df06acbfe2d55650f97ff6616.jpeg https://app.usmall.ru/image/39508152]</t>
+  </si>
+  <si>
+    <t>Мандалорское одеяние для маленьких мальчиков</t>
+  </si>
+  <si>
+    <t>Little Boys Mandalorian Robe</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4808587-little-boys-mandalorian-robe-ame</t>
+  </si>
+  <si>
+    <t>4808587</t>
   </si>
   <si>
     <t>AME</t>
   </si>
   <si>
-    <t>Little Boys Mandalorian Robe</t>
-  </si>
-  <si>
-    <t>Мандалорское одеяние для маленьких мальчиков AME</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4808587-little-boys-mandalorian-robe-ame</t>
-  </si>
-  <si>
-    <t>4808587</t>
-  </si>
-  <si>
-    <t>Завяжите вокруг талииВоротник декольтеОгнестойкий материал.Роскошный плюш, ПолиэстерМожно стирать в машине</t>
+    <t>AME привносит веселье мандалорца в свой образ перед сном с помощью этого халата.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Завяжите вокруг талии&lt;/li&gt;&lt;li&gt;Воротник декольте&lt;/li&gt;&lt;li&gt;Огнестойкий материал.&lt;/li&gt;&lt;li&gt;Роскошный плюш, Полиэстер&lt;/li&gt;&lt;li&gt;Можно стирать в машине&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>AME brings the fun of Mandalorian to his bedtime looks with this robe.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Tie around the waist closure&lt;/li&gt;&lt;li&gt;Collar neckline&lt;/li&gt;&lt;li&gt;Flame resistant&lt;/li&gt;&lt;li&gt;Luxe Plush, Polyester&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[разноцветный]</t>
+  </si>
+  <si>
+    <t>[4 6]</t>
+  </si>
+  <si>
+    <t>разноцветный</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/480/72/22/30685f9b6528e5e22e1862223292f1b9.jpeg]</t>
   </si>
   <si>
-    <t>[Разноцветный (Multi)]</t>
-  </si>
-  <si>
-    <t>[4 6]</t>
+    <t>Одеяние Майнкрафт для маленьких мальчиков</t>
   </si>
   <si>
     <t>Little Boys Minecraft Robe</t>
   </si>
   <si>
-    <t>Одеяние Майнкрафт для маленьких мальчиков AME</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4808473-little-boys-minecraft-robe-ame</t>
   </si>
   <si>
     <t>4808473</t>
   </si>
   <si>
+    <t>В этом халате AME привносит веселье Minecraft в свой образ перед сном.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Завяжите вокруг талии&lt;/li&gt;&lt;li&gt;Воротник декольте&lt;/li&gt;&lt;li&gt;Огнестойкий материал.&lt;/li&gt;&lt;li&gt;Роскошный плюш, Полиэстер&lt;/li&gt;&lt;li&gt;Можно стирать в машине&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>AME brings the fun of Minecraft to his bedtime looks with this robe.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Tie around the waist closure&lt;/li&gt;&lt;li&gt;Collar neckline&lt;/li&gt;&lt;li&gt;Flame resistant&lt;/li&gt;&lt;li&gt;Luxe Plush, Polyester&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[6]</t>
+  </si>
+  <si>
     <t>[https://usmall.ru/image/480/39/88/6a817194d3eb44e98dff7dc5d5c3e383.jpeg]</t>
   </si>
   <si>
+    <t>Мандалорское одеяние для больших мальчиков</t>
+  </si>
+  <si>
     <t>Big Boys Mandalorian Robe</t>
   </si>
   <si>
-    <t>Мандалорское одеяние для больших мальчиков AME</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4807222-big-boys-mandalorian-robe-ame</t>
   </si>
   <si>
@@ -474,12 +521,12 @@
     <t>[8 10]</t>
   </si>
   <si>
+    <t>Одеяние Minecraft для больших мальчиков</t>
+  </si>
+  <si>
     <t>Big Boys Minecraft Robe</t>
   </si>
   <si>
-    <t>Одеяние Minecraft для больших мальчиков AME</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4803988-big-boys-minecraft-robe-ame</t>
   </si>
   <si>
@@ -489,10 +536,10 @@
     <t>[8 10 12]</t>
   </si>
   <si>
-    <t>Boys 4-10 Jurassic World "Dino Stomp" Robe</t>
-  </si>
-  <si>
-    <t>Мальчики 4–10 лет «Мир Юрского периода» &amp;#34;Дино Стомп&amp;#34; Халат Licensed Character</t>
+    <t>Мальчики 4–10 лет «Мир Юрского периода» &amp;#34;Дино Стомп&amp;#34; Халат</t>
+  </si>
+  <si>
+    <t>Boys 4-10 Jurassic World &amp;#34;Dino Stomp&amp;#34; Robe</t>
   </si>
   <si>
     <t>https://usmall.ru/product/4729521-boys-4-10-jurassic-world-34dino-stomp34-robe-licensed-character</t>
@@ -501,34 +548,43 @@
     <t>4729521</t>
   </si>
   <si>
-    <t>Полиэстер В целях безопасности детей одежда должна быть плотно прилегающей или огнестойкой. Это огнеупорная одежда. Машинная стирка Импортные</t>
+    <t>&lt;p&gt;Ему понравится, как Дино топает по дому в уютном и комфортном халате для мальчиков.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Длинный рукав&lt;/li&gt; &lt;li&gt;Открытый фронт&lt;/li&gt; &lt;li&gt;Завязывание&lt;/li&gt; &lt;li&gt;Длина колена&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ТКАНИ И УХОД&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Полиэстер&lt;/li&gt; &lt;li&gt;В целях безопасности детей одежда должна быть плотно прилегающей или огнестойкой. Это огнеупорная одежда.&lt;/li&gt; &lt;li&gt;Машинная стирка&lt;/li&gt; &lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; He'll love Dino Stomping around the house in the cozy comfort of this boys' robe. &lt;/p&gt;&lt;br /&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Long sleeves&lt;/li&gt; &lt;li&gt;Open front&lt;/li&gt; &lt;li&gt;Tie closure&lt;/li&gt; &lt;li&gt;Knee length&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;FABRIC &amp;amp; CARE&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polyester&lt;/li&gt; &lt;li&gt;For children's safety the garment should be snug fitting or flame resistant. This is a flame resistant garment.&lt;/li&gt; &lt;li&gt;Machine wash&lt;/li&gt; &lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[4 8]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/472/95/21/421058ca2a3c1379c5b6a0aeda59d73b.jpeg https://usmall.ru/image/000/00/00/4d2f4b76b7a4396d2ff1dd9b3420d8ea.jpeg]</t>
   </si>
   <si>
-    <t>[4 8]</t>
+    <t>Халат с длинными рукавами и тапочками для мальчиков Big Boy, комплект из 2 предметов</t>
   </si>
   <si>
     <t>Big Boys Long Sleeve Robe with Slippers, 2 Piece Set</t>
   </si>
   <si>
-    <t>Халат с длинными рукавами и тапочками для мальчиков Big Boy, комплект из 2 предметов Max &amp; Olivia</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/4714476-big-boys-long-sleeve-robe-with-slippers-2-piece-set-max-olivia</t>
   </si>
   <si>
     <t>4714476</t>
   </si>
   <si>
-    <t>В комплект входит- 1 халат и 1 пара тапочек.Длинный рукавХалат с поясом и шалевым воротником100% полиэстерМожно стирать в машине</t>
-  </si>
-  <si>
-    <t>Boys 4-10 Marvel The Avengers Black Panther "Panther King" Robe</t>
-  </si>
-  <si>
-    <t>Мальчики 4–10 лет Marvel Мстители Черная пантера &amp;#34;Король пантер&amp;#34; Халат Licensed Character</t>
+    <t>Согрейтесь, отдыхая в этом уютном плюшевом халате из флиса с подходящими тапочками.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;В комплект входит- 1 халат и 1 пара тапочек.&lt;/li&gt;&lt;li&gt;Длинный рукав&lt;/li&gt;&lt;li&gt;Халат с поясом и шалевым воротником&lt;/li&gt;&lt;li&gt;100% полиэстер&lt;/li&gt;&lt;li&gt;Можно стирать в машине&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Keep warm lounging in this cozy, plush fleece robe with matching slippers.&lt;br /&gt;&lt;ul&gt;&lt;li&gt;Set includes- 1 robe and 1 pair of slippers&lt;/li&gt;&lt;li&gt;Long sleeve&lt;/li&gt;&lt;li&gt;Belted robe with shawl collar&lt;/li&gt;&lt;li&gt;100% Polyester&lt;/li&gt;&lt;li&gt;Machine Washable&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[M (8/10) L (12/14) XL (16/18)]</t>
+  </si>
+  <si>
+    <t>Мальчики 4–10 лет Marvel Мстители Черная пантера &amp;#34;Король пантер&amp;#34; Халат</t>
+  </si>
+  <si>
+    <t>Boys 4-10 Marvel The Avengers Black Panther &amp;#34;Panther King&amp;#34; Robe</t>
   </si>
   <si>
     <t>https://usmall.ru/product/4686045-boys-4-10-marvel-the-avengers-black-panther-34panther-king34-robe-licensed-character</t>
@@ -537,222 +593,334 @@
     <t>4686045</t>
   </si>
   <si>
-    <t>Полиэстер Машинная стирка Импортные</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/468/60/45/d406229a8214bce87111c84678e799ae.jpeg https://usmall.ruhttps://app.usmall.ru/image/39641492]</t>
+    <t>&lt;p&gt;Вашему поклоннику Marvel понравится бездельничать в героическом стиле этой мантии Черной пантеры для мальчиков.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Завязывание&lt;/li&gt; &lt;li&gt;Длинный рукав&lt;/li&gt; &lt;li&gt;Длина колена&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ТКАНИ И УХОД&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Полиэстер&lt;/li&gt; &lt;li&gt;Машинная стирка&lt;/li&gt; &lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Your Marvel fan will love lounging in the heroic style of this boys' Black Panther robe. &lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tie closure&lt;/li&gt; &lt;li&gt;Long sleeves&lt;/li&gt; &lt;li&gt;Knee length&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;FABRIC &amp;amp; CARE&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polyester&lt;/li&gt; &lt;li&gt;Machine wash&lt;/li&gt; &lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>[4 6 8]</t>
   </si>
   <si>
+    <t>[https://usmall.ru/image/468/60/45/d406229a8214bce87111c84678e799ae.jpeg https://app.usmall.ru/image/39641492]</t>
+  </si>
+  <si>
+    <t>Халат Cuddl Duds с капюшоном для мальчиков 4–14 лет</t>
+  </si>
+  <si>
+    <t>Boys 4-14 Cuddl Duds Hooded Robe</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4666426-boys-4-14-cuddl-duds-hooded-robe-cuddl-duds</t>
+  </si>
+  <si>
+    <t>4666426</t>
+  </si>
+  <si>
     <t>Cuddl Duds</t>
   </si>
   <si>
-    <t>Boys 4-14 Cuddl Duds Hooded Robe</t>
-  </si>
-  <si>
-    <t>Халат Cuddl Duds с капюшоном для мальчиков 4–14 лет Cuddl Duds</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4666426-boys-4-14-cuddl-duds-hooded-robe-cuddl-duds</t>
-  </si>
-  <si>
-    <t>4666426</t>
+    <t>&lt;p&gt;Этот халат с капюшоном для мальчиков от Cuddl Duds идеально подходит для создания уюта в непринужденные дни отдыха.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Прикрепленный капюшон&lt;/li&gt; &lt;li&gt;2 функциональных кармана&lt;/li&gt; &lt;li&gt;Включает прикрепленный ремень&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ТКАНИ И УХОД&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Полиэстер&lt;/li&gt; &lt;li&gt;Машинная стирка&lt;/li&gt; &lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt; Perfect for keeping cozy on laid-back lounge days, he'll love this boys' hooded robe from Cuddl Duds. &lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Attached hood&lt;/li&gt; &lt;li&gt;2 functional pockets&lt;/li&gt; &lt;li&gt;Includes attached belt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;FABRIC &amp;amp; CARE&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Polyester&lt;/li&gt; &lt;li&gt;Machine wash&lt;/li&gt; &lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[ синий черный красный]</t>
+  </si>
+  <si>
+    <t>[4-6 8-10 12-14]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/466/64/26/05983c3b651413ff990a0bad5cd8116d.jpeg https://usmall.ru/image/000/00/00/4d2f4b76b7a4396d2ff1dd9b3420d8ea.jpeg]</t>
   </si>
   <si>
-    <t>[Черный (Black) Красный (Red Buff Check) Синий (Blue Plaid) Синий (Blue Sports) Teal Gamer]</t>
+    <t>[https://usmall.ru/image/466/64/26/69fdf5ff67410afd6982c97f7f813168.jpeg https://usmall.ru/image/000/00/00/4d2f4b76b7a4396d2ff1dd9b3420d8ea.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/466/64/26/acfa8904864b81116fce9677d46b013a.jpeg https://usmall.ru/image/000/00/00/4d2f4b76b7a4396d2ff1dd9b3420d8ea.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/466/64/26/d4ce375c84f763e3257b65a3ca459adc.jpeg https://usmall.ru/image/000/00/00/4d2f4b76b7a4396d2ff1dd9b3420d8ea.jpeg]</t>
+  </si>
+  <si>
+    <t>Флисовый халат Dino Silhouettes (для малышей/маленьких детей/больших детей)</t>
+  </si>
+  <si>
+    <t>Dino Silhouettes Fleece Robe (Toddler/Little Kids/Big Kids)</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4644024-dino-silhouettes-fleece-robe-toddlerlittle-kidsbig-kids-hatley-kids</t>
+  </si>
+  <si>
+    <t>4644024</t>
   </si>
   <si>
     <t>Hatley Kids</t>
   </si>
   <si>
-    <t>Dino Silhouettes Fleece Robe (Toddler/Little Kids/Big Kids)</t>
-  </si>
-  <si>
-    <t>Флисовый халат Dino Silhouettes (для малышей/маленьких детей/больших детей) Hatley Kids</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4644024-dino-silhouettes-fleece-robe-toddlerlittle-kidsbig-kids-hatley-kids</t>
-  </si>
-  <si>
-    <t>4644024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Длина изделия: 32 дюйма
-</t>
+    <t>&lt;ul&gt;&lt;li&gt;Оберните своего малыша флисовым халатом Hatley® Kids Dino Silhouettes после уютной ванны и держите его в тепле.&lt;/li&gt;
+&lt;li&gt;Вместительная конструкция с капюшоном.&lt;/li&gt;
+&lt;li&gt;Длинный рукав.&lt;/li&gt;
+&lt;li&gt;Пояс с петлей на талии с завязывающимся поясным ремнем.&lt;/li&gt;
+&lt;li&gt;Нижние передние накладные карманы.&lt;/li&gt;
+&lt;li&gt;Сплошной силуэт динозавра.&lt;/li&gt;
+&lt;li&gt;100% полиэстер.&lt;/li&gt;
+&lt;li&gt;Машинная стирка, сушка в стиральной машине.&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;li&gt;Размеры:&lt;ul&gt;&lt;li&gt;Длина изделия: 32 дюйма&lt;/li&gt;
+    &lt;/ul&gt;&lt;/li&gt;
+&lt;li&gt;Измерения продукта были сделаны для размера XL (8-10 Big Kid). Заметьте, пожалуйста, что измерения могут быть разной величины.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Wrap your little one in the  Hatley® Kids Dino Silhouettes Fleece Robe after a cozy bath and keep them warm.&lt;/li&gt;
+&lt;li&gt;Roomy hooded construction.&lt;/li&gt;
+&lt;li&gt;Long sleeves.&lt;/li&gt;
+&lt;li&gt;Belt loop waist with tie-up waistbelt.&lt;/li&gt;
+&lt;li&gt;Lower front patch pockets.&lt;/li&gt;
+&lt;li&gt;Allover dino silhouette print.&lt;/li&gt;
+&lt;li&gt;100% polyester.&lt;/li&gt;
+&lt;li&gt;Machine wash, tumble dry.&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;li&gt;Measurements:
+&lt;ul&gt;&lt;li&gt; Length: 32 in&lt;/li&gt;
+    &lt;/ul&gt;&lt;/li&gt;
+&lt;li&gt;Product measurements were taken using size XL (8-10 Big Kid). Please note that measurements may vary by size.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[LG (6-7 Little Kid) One Size SM (2-3 Toddler) One Size XL (8-10 Big Kid) One Size MD (4-5 Little Kid) One Size]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/464/40/24/62a25f9ae497c89ea21f57639c863de2.jpeg]</t>
   </si>
   <si>
-    <t>Полиэстер, Флис</t>
-  </si>
-  <si>
-    <t>С принтом</t>
-  </si>
-  <si>
-    <t>Boys 4-12 DC Comics Batman Robe &amp; Slippers Set</t>
-  </si>
-  <si>
-    <t>Мальчики 4-12 DC Comics Batman халат и тапочки Licensed Character</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/4299806-boys-4-12-dc-comics-batman-robe-slippers-set-licensed-character</t>
-  </si>
-  <si>
-    <t>4299806</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/429/98/06/7d19ef4f728ef7eedb517202fd65dda3.jpeg https://usmall.ruhttps://app.usmall.ru/image/40257152 https://usmall.ruhttps://app.usmall.ru/image/34973020 https://usmall.ruhttps://app.usmall.ru/image/34973019 https://usmall.ruhttps://app.usmall.ru/image/34973018 https://usmall.ruhttps://app.usmall.ru/image/34973017]</t>
-  </si>
-  <si>
-    <t>[Черный (Black)]</t>
-  </si>
-  <si>
-    <t>Девочки</t>
+    <t>Комплект из 2 комплектов пижам Baby Boy Carter's</t>
+  </si>
+  <si>
+    <t>Baby Boy Carter's 2-Pack Sleeper Gowns</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/4298853-baby-boy-carters-2-pack-sleeper-gowns-carters</t>
+  </si>
+  <si>
+    <t>4298853</t>
+  </si>
+  <si>
+    <t>Carter's</t>
+  </si>
+  <si>
+    <t>&lt;br /&gt;&lt;p&gt;Дополните гардероб своего малыша набором из двух комплектов пижам Carter's.&lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;ОСОБЕННОСТИ ПРОДУКТА&lt;/p&gt;&lt;ul&gt;&lt;li&gt;2 штуки в наборе&lt;/li&gt; &lt;li&gt;Вырез-конверт и планка на пуговицах&lt;/li&gt; &lt;li&gt;Длинный рукав&lt;/li&gt; &lt;li&gt;Раскладные манжеты&lt;/li&gt; &lt;li&gt;Подол&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ТКАНИ И УХОД&lt;/p&gt;&lt;ul&gt;&lt;li&gt;хлопок&lt;/li&gt; &lt;li&gt;Машинная стирка&lt;/li&gt; &lt;li&gt;Импортные&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;ОСОБЕННОСТИ УСТОЙЧИВОГО РАЗВИТИЯ&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Проверено на вредные вещества&lt;/li&gt;&lt;li&gt;СТАНДАРТ 100 СЕРТИФИЦИРОВАНО OEKO-TEX®&lt;/li&gt; &lt;li&gt;Сертификат № 20.HUS.39362&lt;/li&gt; &lt;li&gt;Институт испытаний: Институт испытаний текстиля Хоэнштайна&lt;/li&gt;&lt;li&gt;www.oeko-tex.com/standard100&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;br /&gt;&lt;p&gt; Complete your little one's wardrobe with these Carter's 2-Pack Sleeper Gowns. &lt;/p&gt;&lt;br /&gt;&lt;p&gt;&lt;/p&gt;&lt;br /&gt;&lt;p&gt;PRODUCT FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;2-pack&lt;/li&gt; &lt;li&gt;Envelope neck &amp;amp; button placket&lt;/li&gt; &lt;li&gt;Long sleeves&lt;/li&gt; &lt;li&gt;Foldover cuffs&lt;/li&gt; &lt;li&gt;Cinched hem&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;FABRIC &amp;amp; CARE&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Cotton&lt;/li&gt; &lt;li&gt;Machine wash&lt;/li&gt; &lt;li&gt;Imported&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;SUSTAINABILITY FEATURES&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Tested for harmful substances&lt;/li&gt;&lt;li&gt;STANDARD 100 by OEKO-TEXÂ® CERTIFIED&lt;/li&gt; &lt;li&gt;Certification No. 20.HUS.39362&lt;/li&gt; &lt;li&gt;Testing Institute: Hohenstein Textile Testing Institute&lt;/li&gt;&lt;li&gt;www.oeko-tex.com/standard100&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[NEWBORN 3 MONTHS]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/429/88/53/022c49a47338728c74360fc35a6c13c6.jpeg https://app.usmall.ru/image/39607526 https://usmall.ru/image/000/00/00/2d562595e37b7d3146b8d9c0c1c335af.jpeg https://usmall.ru/image/000/00/00/8d03b188a464fe7bf3d398929f027a32.jpeg https://usmall.ru/image/000/00/00/2e450948e39957b366e84a73f347d88f.jpeg]</t>
+  </si>
+  <si>
+    <t>Уютный халат с животными (для больших детей)</t>
+  </si>
+  <si>
+    <t>Cozy Animal Robe (Big Kids)</t>
+  </si>
+  <si>
+    <t>https://usmall.ru/product/3336498-cozy-animal-robe-big-kids-llbean</t>
+  </si>
+  <si>
+    <t>3336498</t>
   </si>
   <si>
     <t>L.L.Bean</t>
   </si>
   <si>
-    <t>Cozy Animal Robe (Big Kids)</t>
-  </si>
-  <si>
-    <t>Уютный халат с животными (для больших детей) L.L.Bean</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/3336498-cozy-animal-robe-big-kids-llbean</t>
-  </si>
-  <si>
-    <t>3336498</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Подарите своему ребенку уют от подбородка до голени в этом невероятно мягком, плюшевом и удобном халате LL Bean™ Cosy Animal Robe (Big Kids).
-Свободный крой.
-Графические детали животных на капюшоне.
-Уютный капюшон зверька.
-Глубокие передние карманы.
-Притачной пояс.
-Ткань соответствует федеральным требованиям безопасности для детской одежды для сна.
-Сверхмягкая конструкция из 100% полиэстера с высоким ворсом и начесом с обеих сторон.
-Можно стирать в машине.
-Импортные.
-</t>
+    <t>&lt;ul&gt;&lt;li&gt;Подарите своему ребенку уют от подбородка до голени в этом невероятно мягком, плюшевом и удобном халате LL Bean™ Cosy Animal Robe (Big Kids).&lt;/li&gt;
+&lt;li&gt;Свободный крой.&lt;/li&gt;
+&lt;li&gt;Графические детали животных на капюшоне.&lt;/li&gt;
+&lt;li&gt;Уютный капюшон зверька.&lt;/li&gt;
+&lt;li&gt;Глубокие передние карманы.&lt;/li&gt;
+&lt;li&gt;Притачной пояс.&lt;/li&gt;
+&lt;li&gt;Ткань соответствует федеральным требованиям безопасности для детской одежды для сна.&lt;/li&gt;
+&lt;li&gt;Сверхмягкая конструкция из 100% полиэстера с высоким ворсом и начесом с обеих сторон.&lt;/li&gt;
+&lt;li&gt;Можно стирать в машине.&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Keep your kid cozy from chin to shin in this incredibly soft, plush, and comfortable L.L. Bean™ Cozy Animal Robe (Big Kids).&lt;/li&gt;
+&lt;li&gt;Relaxed fit.&lt;/li&gt;
+&lt;li&gt;Animal graphic details on the hood.&lt;/li&gt;
+&lt;li&gt;Cozy critter hood. &lt;/li&gt;
+&lt;li&gt;Deep front pockets.&lt;/li&gt;
+&lt;li&gt;Stitched-down belt.&lt;/li&gt;
+&lt;li&gt;Fabric meets federal safety requirements for children's sleepwear.&lt;/li&gt;
+&lt;li&gt;Super-soft, high-pile, both side brushed 100% polyester construction.&lt;/li&gt;
+&lt;li&gt;Machine washable.&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[синий розовый коричневый]</t>
+  </si>
+  <si>
+    <t>[SM (8 Big Kid) One Size MD (10-12 Big Kid) One Size LG (14-16 Big Kid) One Size XL (18 Big Kid) One Size]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/333/64/98/dccf74fa1c3db42db12b2e540edd79cf.jpeg https://usmall.ru/image/333/64/98/fd8441316e47d3912a6502b6a8d44eb9.jpeg]</t>
   </si>
   <si>
-    <t>[Розовый (Mauve Berry) Коричневый (Dark Barley) Синий (Bright Blue)]</t>
+    <t>[https://usmall.ru/image/333/64/98/27243be246d3869d59b1cf3aaa94fbb7.jpeg https://usmall.ru/image/333/64/98/45b85ca2873fef98924c23317f6a74b7.jpeg]</t>
+  </si>
+  <si>
+    <t>коричневый</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/38076144 https://app.usmall.ru/image/38076146]</t>
+  </si>
+  <si>
+    <t>Флисовый халат (маленькие дети)</t>
   </si>
   <si>
     <t>Fleece Robe (Little Kids)</t>
   </si>
   <si>
-    <t>Флисовый халат (маленькие дети) L.L.Bean</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/3214979-fleece-robe-little-kids-llbean</t>
   </si>
   <si>
     <t>3214979</t>
   </si>
   <si>
-    <t xml:space="preserve">Устройтесь поудобнее в этом уютном флисовом халате LL Bean™. Этот толстый флисовый халат отлично смотрится после стирки.
-Изготовлен из ультрамягкой флисовой ткани.
-Плюшевый воротник поднимается вверх, чтобы предотвратить сквозняки.
-Глубокие передние карманы.
-100% полиэстер флис.
-Машинная стирка и сушка.
-Импортные.
-</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/321/49/79/81d5deed9f7df1ea4f10694e6686a6c2.jpeg]</t>
-  </si>
-  <si>
-    <t>[Красный (Apple Red) Зеленый (Emerald Spruce) Синий (Island Blue) Синий (Blue) Пурпурный (Plum Grape)]</t>
+    <t>&lt;ul&gt;&lt;li&gt;Устройтесь поудобнее в этом уютном флисовом халате LL Bean™. Этот толстый флисовый халат отлично смотрится после стирки.&lt;/li&gt;
+&lt;li&gt;Изготовлен из ультрамягкой флисовой ткани.&lt;/li&gt;
+&lt;li&gt;Плюшевый воротник поднимается вверх, чтобы предотвратить сквозняки.&lt;/li&gt;
+&lt;li&gt;Глубокие передние карманы.&lt;/li&gt;
+&lt;li&gt;100% полиэстер флис.&lt;/li&gt;
+&lt;li&gt;Машинная стирка и сушка.&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Snuggle up and feel comfy in this cozy L.L Bean™  Fleece Robe. This thick fleece robe looks great wash after wash.&lt;/li&gt;
+&lt;li&gt;Made of ultra-plush fleece fabric.&lt;/li&gt;
+&lt;li&gt;Plush collar turns up to stop drafts.&lt;/li&gt;
+&lt;li&gt;Deep front pockets.&lt;/li&gt;
+&lt;li&gt;100% polyester fleece.&lt;/li&gt;
+&lt;li&gt;Machine wash and dry.&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[синий красный Пурпурный зеленый]</t>
+  </si>
+  <si>
+    <t>[SM (4 Little Kid) One Size MD (5-6 Little Kid) One Size LG (6X-7 Little Kid) One Size]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/79/64c3912170002fee2d4ead154ece1196.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/79/79c702a0cd0fa64ca79eb2eb8a38d416.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/38075831]</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/26060814]</t>
+  </si>
+  <si>
+    <t>Флисовый халат (для больших детей)</t>
   </si>
   <si>
     <t>Fleece Robe (Big Kids)</t>
   </si>
   <si>
-    <t>Флисовый халат (для больших детей) L.L.Bean</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/3214975-fleece-robe-big-kids-llbean</t>
   </si>
   <si>
     <t>3214975</t>
   </si>
   <si>
-    <t xml:space="preserve">Удобный и теплый флисовый халат LL Bean™ из толстого ультраплюшевого флиса.
-Плюшевый воротник поднимается вверх, чтобы предотвратить сквозняки.
-На талии крепится флисовый пояс.
-Глубокие передние карманы.
-100% полиэстер флис.
-Можно стирать в машине.
-Импортные.
-</t>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/321/49/75/e4dd30163f3ef7f24e1d097ba09fa338.jpeg]</t>
-  </si>
-  <si>
-    <t>Gap Factory</t>
-  </si>
-  <si>
-    <t>Toddler Brannan Bear Hoodie Robe</t>
-  </si>
-  <si>
-    <t>Toddler Brannan Bear Hoodie Robe Gap Factory</t>
-  </si>
-  <si>
-    <t>https://usmall.ru/product/3129308-toddler-brannan-bear-hoodie-robe-gap-factory</t>
-  </si>
-  <si>
-    <t>3129308</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>[https://usmall.ru/image/312/93/08/3028eaf6c3405547b01c42eebbb6d95d.jpeg]</t>
-  </si>
-  <si>
-    <t>[Слоновая кость (Creme Brule)]</t>
+    <t>&lt;ul&gt;&lt;li&gt;Удобный и теплый флисовый халат LL Bean™ из толстого ультраплюшевого флиса.&lt;/li&gt;
+&lt;li&gt;Плюшевый воротник поднимается вверх, чтобы предотвратить сквозняки.&lt;/li&gt;
+&lt;li&gt;На талии крепится флисовый пояс.&lt;/li&gt;
+&lt;li&gt;Глубокие передние карманы.&lt;/li&gt;
+&lt;li&gt;100% полиэстер флис.&lt;/li&gt;
+&lt;li&gt;Можно стирать в машине.&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Featuring a thick ultra-plush fleece, the L.L Bean™ Fleece Robe is comfy and warm.&lt;/li&gt;
+&lt;li&gt;Plush collar turns up to stop drafts.&lt;/li&gt;
+&lt;li&gt;Fleece belt attached to the waist.&lt;/li&gt;
+&lt;li&gt;Deep front pockets.&lt;/li&gt;
+&lt;li&gt;100% polyester fleece.&lt;/li&gt;
+&lt;li&gt;Machine washable.&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/75/4293697fc68c6318bfc4734cf41b224e.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/75/51eea0f33b49bb74788664f9a2dbcd84.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/75/3ec61b72c412febd4f760286da6f35d5.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/321/49/75/2ab9ac621f0be3ee6e3535fe869ea92e.jpeg]</t>
+  </si>
+  <si>
+    <t>Уютный халат с животными (маленькие дети)</t>
   </si>
   <si>
     <t>Cozy Animal Robe (Little Kids)</t>
   </si>
   <si>
-    <t>Уютный халат с животными (маленькие дети) L.L.Bean</t>
-  </si>
-  <si>
     <t>https://usmall.ru/product/2988329-cozy-animal-robe-little-kids-llbean</t>
   </si>
   <si>
     <t>2988329</t>
   </si>
   <si>
-    <t xml:space="preserve">Устройтесь поудобнее со своим малышом в их очаровательном комбинезоне LLBean™ Cozy Animal Robe.
-Этот халат, изготовленный из очень мягкого полиэстера, имеет капюшон с ушками в виде животных, глубокие передние карманы и пояс с завязками на талии.
-Этот халат не распространяет горение и соответствует требованиям безопасности для детской одежды для сна.
-Легко тянуть на строительство.
-100% полиэстер.
-Машинная стирка, сушка в стиральной машине.
-Импортные.
-</t>
+    <t>&lt;ul&gt;&lt;li&gt;Устройтесь поудобнее со своим малышом в их очаровательном комбинезоне LLBean™ Cozy Animal Robe.&lt;/li&gt;
+&lt;li&gt;Этот халат, изготовленный из очень мягкого полиэстера, имеет капюшон с ушками в виде животных, глубокие передние карманы и пояс с завязками на талии.&lt;/li&gt;
+&lt;li&gt;Этот халат не распространяет горение и соответствует требованиям безопасности для детской одежды для сна.&lt;/li&gt;
+&lt;li&gt;Легко тянуть на строительство.&lt;/li&gt;
+&lt;li&gt;100% полиэстер.&lt;/li&gt;
+&lt;li&gt;Машинная стирка, сушка в стиральной машине.&lt;/li&gt;
+&lt;li&gt;Импортные.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Snuggle up with your little one in their adorable L.L.Bean™ Cozy Animal Robe.&lt;/li&gt;
+&lt;li&gt;Crafted from a super soft polyester, this robe features an animal designed hood with ears, deep front pockets, and a self tie belt at the waist. &lt;/li&gt;
+&lt;li&gt;This robe is flame retardant and meets safety requirements for children's sleepwear.&lt;/li&gt;
+&lt;li&gt;Easy pull on construction.&lt;/li&gt;
+&lt;li&gt;100% polyester.&lt;/li&gt;
+&lt;li&gt;Machine wash, tumble dry.&lt;/li&gt;
+&lt;li&gt;Imported.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>[синий розовый серый коричневый]</t>
   </si>
   <si>
     <t>[https://usmall.ru/image/298/83/29/9c885434a9326e6f78506758791b4d47.jpeg https://usmall.ru/image/298/83/29/d1a4405f9bab6d07d4f1e175bec8f24e.jpeg]</t>
   </si>
   <si>
-    <t>[Серый (Mineral Gray) Розовый (Mauve Berry) Коричневый (Dark Barley) Синий (Bright Blue)]</t>
+    <t>[https://usmall.ru/image/298/83/29/bc57aad91ed2850cc7630c68c6e5a278.jpeg https://usmall.ru/image/298/83/29/55a4d521a9f3e62a1534587d2a869920.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://usmall.ru/image/298/83/29/8eaae1529cbceddb299cb770167a9b7a.jpeg]</t>
+  </si>
+  <si>
+    <t>[https://app.usmall.ru/image/38070272 https://app.usmall.ru/image/38070274]</t>
   </si>
 </sst>
 </file>
@@ -1105,22 +1273,40 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Q1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="S1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="T1" t="s">
-        <v>75</v>
+        <v>98</v>
+      </c>
+      <c r="U1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" t="s">
+        <v>104</v>
+      </c>
+      <c r="W1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="2">
@@ -1128,52 +1314,46 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
       </c>
       <c r="J2">
         <v>7040</v>
       </c>
       <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -1181,52 +1361,46 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <v>3640</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -1234,43 +1408,46 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <v>4520</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="Q4" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4">
-        <v>6280</v>
-      </c>
-      <c r="K4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -1278,46 +1455,46 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>6280</v>
+      </c>
+      <c r="K5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="E5" t="s">
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
+      <c r="Q5" t="s">
         <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5">
-        <v>4400</v>
-      </c>
-      <c r="K5" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6">
@@ -1325,46 +1502,46 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J6">
         <v>4400</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
@@ -1372,46 +1549,49 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J7">
         <v>4400</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7" t="s">
-        <v>29</v>
+        <v>66</v>
+      </c>
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -1419,49 +1599,49 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8">
+        <v>4400</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" t="s">
+      <c r="N8" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="O8" t="s">
         <v>67</v>
       </c>
-      <c r="G8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="R8" t="s">
         <v>69</v>
-      </c>
-      <c r="I8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8">
-        <v>4520</v>
-      </c>
-      <c r="K8" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" t="s">
-        <v>71</v>
-      </c>
-      <c r="M8" t="s">
-        <v>72</v>
-      </c>
-      <c r="N8" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9">
@@ -1469,43 +1649,46 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J9">
         <v>4520</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="N9" t="s">
-        <v>40</v>
+        <v>76</v>
+      </c>
+      <c r="R9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="10">
@@ -1513,49 +1696,46 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J10">
         <v>5530</v>
       </c>
       <c r="K10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="M10" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
-      </c>
-      <c r="P10" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>31</v>
+        <v>85</v>
+      </c>
+      <c r="R10" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11">
@@ -1563,43 +1743,64 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J11">
         <v>5460</v>
       </c>
       <c r="K11" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L11" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" t="s">
+        <v>94</v>
+      </c>
+      <c r="N11" t="s">
+        <v>95</v>
+      </c>
+      <c r="P11" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>103</v>
+      </c>
+      <c r="R11" t="s">
+        <v>102</v>
+      </c>
+      <c r="S11" t="s">
+        <v>97</v>
+      </c>
+      <c r="T11" t="s">
         <v>99</v>
       </c>
-      <c r="M11" t="s">
-        <v>100</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="U11" t="s">
         <v>101</v>
+      </c>
+      <c r="V11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12">
@@ -1607,43 +1808,64 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J12">
         <v>5460</v>
       </c>
       <c r="K12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N12" t="s">
+        <v>95</v>
+      </c>
+      <c r="P12" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>103</v>
+      </c>
+      <c r="R12" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" t="s">
+        <v>97</v>
+      </c>
+      <c r="T12" t="s">
         <v>99</v>
       </c>
-      <c r="M12" t="s">
-        <v>100</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="U12" t="s">
         <v>101</v>
+      </c>
+      <c r="V12" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13">
@@ -1651,43 +1873,64 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H13" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J13">
         <v>5460</v>
       </c>
       <c r="K13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" t="s">
+        <v>94</v>
+      </c>
+      <c r="N13" t="s">
+        <v>95</v>
+      </c>
+      <c r="P13" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>103</v>
+      </c>
+      <c r="R13" t="s">
+        <v>102</v>
+      </c>
+      <c r="S13" t="s">
+        <v>97</v>
+      </c>
+      <c r="T13" t="s">
         <v>99</v>
       </c>
-      <c r="M13" t="s">
-        <v>100</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="U13" t="s">
         <v>101</v>
+      </c>
+      <c r="V13" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14">
@@ -1695,43 +1938,64 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J14">
         <v>5460</v>
       </c>
       <c r="K14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L14" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" t="s">
+        <v>95</v>
+      </c>
+      <c r="P14" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>103</v>
+      </c>
+      <c r="R14" t="s">
+        <v>102</v>
+      </c>
+      <c r="S14" t="s">
+        <v>97</v>
+      </c>
+      <c r="T14" t="s">
         <v>99</v>
       </c>
-      <c r="M14" t="s">
-        <v>100</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="U14" t="s">
         <v>101</v>
+      </c>
+      <c r="V14" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15">
@@ -1739,43 +2003,64 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F15" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J15">
         <v>5460</v>
       </c>
       <c r="K15" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L15" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N15" t="s">
+        <v>95</v>
+      </c>
+      <c r="P15" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>103</v>
+      </c>
+      <c r="R15" t="s">
+        <v>102</v>
+      </c>
+      <c r="S15" t="s">
+        <v>97</v>
+      </c>
+      <c r="T15" t="s">
         <v>99</v>
       </c>
-      <c r="M15" t="s">
-        <v>100</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="U15" t="s">
         <v>101</v>
+      </c>
+      <c r="V15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16">
@@ -1783,43 +2068,64 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J16">
         <v>5460</v>
       </c>
       <c r="K16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="L16" t="s">
+        <v>93</v>
+      </c>
+      <c r="M16" t="s">
+        <v>94</v>
+      </c>
+      <c r="N16" t="s">
+        <v>95</v>
+      </c>
+      <c r="P16" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>103</v>
+      </c>
+      <c r="R16" t="s">
+        <v>102</v>
+      </c>
+      <c r="S16" t="s">
+        <v>97</v>
+      </c>
+      <c r="T16" t="s">
         <v>99</v>
       </c>
-      <c r="M16" t="s">
-        <v>100</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="U16" t="s">
         <v>101</v>
+      </c>
+      <c r="V16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17">
@@ -1827,43 +2133,64 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17">
+        <v>5460</v>
+      </c>
+      <c r="K17" t="s">
+        <v>92</v>
+      </c>
+      <c r="L17" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" t="s">
+        <v>95</v>
+      </c>
+      <c r="P17" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>103</v>
+      </c>
+      <c r="R17" t="s">
         <v>102</v>
       </c>
-      <c r="E17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="S17" t="s">
+        <v>97</v>
+      </c>
+      <c r="T17" t="s">
+        <v>99</v>
+      </c>
+      <c r="U17" t="s">
+        <v>101</v>
+      </c>
+      <c r="V17" t="s">
         <v>105</v>
-      </c>
-      <c r="H17" t="s">
-        <v>106</v>
-      </c>
-      <c r="I17" t="s">
-        <v>103</v>
-      </c>
-      <c r="J17">
-        <v>3520</v>
-      </c>
-      <c r="K17" t="s">
-        <v>107</v>
-      </c>
-      <c r="L17" t="s">
-        <v>108</v>
-      </c>
-      <c r="M17" t="s">
-        <v>109</v>
-      </c>
-      <c r="N17" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="18">
@@ -1871,43 +2198,46 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J18">
         <v>3520</v>
       </c>
       <c r="K18" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="L18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M18" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="N18" t="s">
-        <v>118</v>
+        <v>112</v>
+      </c>
+      <c r="R18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19">
@@ -1915,43 +2245,46 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="J19">
         <v>3520</v>
       </c>
       <c r="K19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L19" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M19" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="N19" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="W19" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="20">
@@ -1959,43 +2292,46 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G20" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="I20" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="J20">
         <v>3520</v>
       </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M20" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
       <c r="N20" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="21">
@@ -2003,49 +2339,46 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
+        <v>128</v>
+      </c>
+      <c r="G21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" t="s">
+        <v>110</v>
+      </c>
+      <c r="J21">
+        <v>3520</v>
+      </c>
+      <c r="K21" t="s">
+        <v>131</v>
+      </c>
+      <c r="L21" t="s">
+        <v>131</v>
+      </c>
+      <c r="M21" t="s">
+        <v>132</v>
+      </c>
+      <c r="N21" t="s">
+        <v>126</v>
+      </c>
+      <c r="U21" t="s">
         <v>133</v>
-      </c>
-      <c r="E21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" t="s">
-        <v>137</v>
-      </c>
-      <c r="I21" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21">
-        <v>7290</v>
-      </c>
-      <c r="K21" t="s">
-        <v>138</v>
-      </c>
-      <c r="L21" t="s">
-        <v>139</v>
-      </c>
-      <c r="M21" t="s">
-        <v>140</v>
-      </c>
-      <c r="N21" t="s">
-        <v>141</v>
-      </c>
-      <c r="P21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22">
@@ -2053,49 +2386,46 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="H22" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J22">
         <v>7290</v>
       </c>
       <c r="K22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L22" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="M22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N22" t="s">
-        <v>40</v>
-      </c>
-      <c r="P22" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>31</v>
+        <v>142</v>
+      </c>
+      <c r="X22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23">
@@ -2103,49 +2433,46 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" t="s">
+        <v>146</v>
+      </c>
+      <c r="G23" t="s">
         <v>147</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>148</v>
       </c>
-      <c r="G23" t="s">
-        <v>149</v>
-      </c>
-      <c r="H23" t="s">
-        <v>150</v>
-      </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="J23">
         <v>7290</v>
       </c>
       <c r="K23" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="L23" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="M23" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N23" t="s">
         <v>151</v>
       </c>
-      <c r="P23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>31</v>
+      <c r="X23" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="24">
@@ -2153,49 +2480,46 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="J24">
         <v>7290</v>
       </c>
       <c r="K24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L24" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="M24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N24" t="s">
-        <v>156</v>
-      </c>
-      <c r="P24" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>31</v>
+        <v>157</v>
+      </c>
+      <c r="X24" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25">
@@ -2203,43 +2527,46 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F25" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G25" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I25" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="J25">
-        <v>2640</v>
+        <v>7290</v>
       </c>
       <c r="K25" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="L25" t="s">
+        <v>150</v>
+      </c>
+      <c r="M25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N25" t="s">
         <v>162</v>
       </c>
-      <c r="M25" t="s">
-        <v>140</v>
-      </c>
-      <c r="N25" t="s">
-        <v>163</v>
+      <c r="X25" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26">
@@ -2247,49 +2574,46 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" t="s">
         <v>164</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>165</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>166</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26">
+        <v>2640</v>
+      </c>
+      <c r="K26" t="s">
         <v>167</v>
       </c>
-      <c r="I26" t="s">
-        <v>164</v>
-      </c>
-      <c r="J26">
-        <v>5530</v>
-      </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>168</v>
       </c>
-      <c r="L26" t="s">
-        <v>91</v>
-      </c>
       <c r="M26" t="s">
-        <v>92</v>
+        <v>141</v>
       </c>
       <c r="N26" t="s">
-        <v>40</v>
-      </c>
-      <c r="P26" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>31</v>
+        <v>169</v>
+      </c>
+      <c r="X26" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="27">
@@ -2297,43 +2621,46 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F27" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="G27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H27" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I27" t="s">
-        <v>169</v>
+        <v>82</v>
       </c>
       <c r="J27">
-        <v>2640</v>
+        <v>5530</v>
       </c>
       <c r="K27" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L27" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M27" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="N27" t="s">
-        <v>175</v>
+        <v>177</v>
+      </c>
+      <c r="R27" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28">
@@ -2341,43 +2668,46 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G28" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I28" t="s">
-        <v>177</v>
+        <v>50</v>
       </c>
       <c r="J28">
-        <v>2520</v>
+        <v>2640</v>
       </c>
       <c r="K28" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="L28" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M28" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="N28" t="s">
-        <v>40</v>
+        <v>184</v>
+      </c>
+      <c r="X28" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="29">
@@ -2385,43 +2715,55 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E29" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="F29" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="G29" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="H29" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="I29" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="J29">
         <v>2520</v>
       </c>
       <c r="K29" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="L29" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="M29" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="N29" t="s">
-        <v>40</v>
+        <v>194</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>198</v>
+      </c>
+      <c r="R29" t="s">
+        <v>196</v>
+      </c>
+      <c r="W29" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="30">
@@ -2429,43 +2771,55 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="F30" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="G30" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="H30" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="I30" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="J30">
         <v>2520</v>
       </c>
       <c r="K30" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="L30" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="M30" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="N30" t="s">
-        <v>40</v>
+        <v>194</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>198</v>
+      </c>
+      <c r="R30" t="s">
+        <v>196</v>
+      </c>
+      <c r="W30" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="31">
@@ -2473,49 +2827,55 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E31" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F31" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G31" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="I31" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="J31">
-        <v>5740</v>
+        <v>2520</v>
       </c>
       <c r="K31" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L31" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="M31" t="s">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="N31" t="s">
-        <v>40</v>
-      </c>
-      <c r="S31" t="s">
-        <v>190</v>
-      </c>
-      <c r="T31" t="s">
-        <v>191</v>
+        <v>194</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>198</v>
+      </c>
+      <c r="R31" t="s">
+        <v>196</v>
+      </c>
+      <c r="W31" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="32">
@@ -2523,560 +2883,644 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E32" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="F32" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="G32" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="H32" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="I32" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="J32">
-        <v>6280</v>
+        <v>5740</v>
       </c>
       <c r="K32" t="s">
-        <v>49</v>
+        <v>204</v>
       </c>
       <c r="L32" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="M32" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="N32" t="s">
-        <v>40</v>
+        <v>206</v>
+      </c>
+      <c r="R32" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E33" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="F33" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="G33" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="H33" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="I33" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="J33">
-        <v>6900</v>
+        <v>1960</v>
       </c>
       <c r="K33" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="L33" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="M33" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="N33" t="s">
-        <v>40</v>
-      </c>
-      <c r="S33" t="s">
-        <v>74</v>
+        <v>215</v>
+      </c>
+      <c r="X33" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="F34" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="G34" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="H34" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="I34" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="J34">
         <v>6900</v>
       </c>
       <c r="K34" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="L34" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="M34" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="N34" t="s">
-        <v>40</v>
-      </c>
-      <c r="S34" t="s">
-        <v>74</v>
+        <v>225</v>
+      </c>
+      <c r="R34" t="s">
+        <v>226</v>
+      </c>
+      <c r="T34" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="F35" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="G35" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="H35" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="I35" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="J35">
         <v>6900</v>
       </c>
       <c r="K35" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
       <c r="L35" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
       <c r="M35" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="N35" t="s">
-        <v>40</v>
-      </c>
-      <c r="S35" t="s">
-        <v>74</v>
+        <v>225</v>
+      </c>
+      <c r="R35" t="s">
+        <v>226</v>
+      </c>
+      <c r="T35" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="F36" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G36" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="H36" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="I36" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="J36">
-        <v>5650</v>
+        <v>6900</v>
       </c>
       <c r="K36" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="L36" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="M36" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="N36" t="s">
-        <v>40</v>
-      </c>
-      <c r="S36" t="s">
-        <v>190</v>
+        <v>225</v>
+      </c>
+      <c r="R36" t="s">
+        <v>226</v>
+      </c>
+      <c r="T36" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="F37" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="G37" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="H37" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="I37" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="J37">
-        <v>5650</v>
+        <v>5590</v>
       </c>
       <c r="K37" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="L37" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="M37" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N37" t="s">
-        <v>40</v>
+        <v>237</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>238</v>
+      </c>
+      <c r="R37" t="s">
+        <v>241</v>
       </c>
       <c r="S37" t="s">
-        <v>190</v>
+        <v>239</v>
+      </c>
+      <c r="U37" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="F38" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="G38" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="H38" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="I38" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="J38">
-        <v>5650</v>
+        <v>5590</v>
       </c>
       <c r="K38" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="L38" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="M38" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N38" t="s">
-        <v>40</v>
+        <v>237</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>238</v>
+      </c>
+      <c r="R38" t="s">
+        <v>241</v>
       </c>
       <c r="S38" t="s">
-        <v>190</v>
+        <v>239</v>
+      </c>
+      <c r="U38" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E39" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="F39" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="G39" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="H39" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="I39" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="J39">
-        <v>5650</v>
+        <v>5590</v>
       </c>
       <c r="K39" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="L39" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="M39" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N39" t="s">
-        <v>40</v>
+        <v>237</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>238</v>
+      </c>
+      <c r="R39" t="s">
+        <v>241</v>
       </c>
       <c r="S39" t="s">
-        <v>190</v>
+        <v>239</v>
+      </c>
+      <c r="U39" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E40" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="F40" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="G40" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="H40" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="I40" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J40">
-        <v>5650</v>
+        <v>5590</v>
       </c>
       <c r="K40" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="L40" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="M40" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N40" t="s">
-        <v>40</v>
+        <v>237</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>238</v>
+      </c>
+      <c r="R40" t="s">
+        <v>241</v>
       </c>
       <c r="S40" t="s">
-        <v>190</v>
+        <v>239</v>
+      </c>
+      <c r="U40" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="F41" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="G41" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="H41" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="I41" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J41">
         <v>5650</v>
       </c>
       <c r="K41" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="L41" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="M41" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N41" t="s">
-        <v>40</v>
+        <v>225</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>250</v>
+      </c>
+      <c r="R41" t="s">
+        <v>249</v>
       </c>
       <c r="S41" t="s">
-        <v>190</v>
+        <v>251</v>
+      </c>
+      <c r="U41" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="F42" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="G42" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="H42" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="I42" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J42">
         <v>5650</v>
       </c>
       <c r="K42" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="L42" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="M42" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N42" t="s">
-        <v>40</v>
+        <v>225</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>250</v>
+      </c>
+      <c r="R42" t="s">
+        <v>249</v>
       </c>
       <c r="S42" t="s">
-        <v>190</v>
+        <v>251</v>
+      </c>
+      <c r="U42" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
       <c r="F43" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="G43" t="s">
-        <v>216</v>
+        <v>244</v>
       </c>
       <c r="H43" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="I43" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="J43">
         <v>5650</v>
       </c>
       <c r="K43" t="s">
-        <v>218</v>
+        <v>246</v>
       </c>
       <c r="L43" t="s">
-        <v>219</v>
+        <v>247</v>
       </c>
       <c r="M43" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="N43" t="s">
-        <v>40</v>
+        <v>225</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>250</v>
+      </c>
+      <c r="R43" t="s">
+        <v>249</v>
       </c>
       <c r="S43" t="s">
-        <v>190</v>
+        <v>251</v>
+      </c>
+      <c r="U43" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="44">
@@ -3084,231 +3528,279 @@
         <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>220</v>
+        <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="F44" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="G44" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="H44" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
       <c r="I44" t="s">
         <v>221</v>
       </c>
       <c r="J44">
-        <v>2510</v>
+        <v>5650</v>
       </c>
       <c r="K44" t="s">
+        <v>246</v>
+      </c>
+      <c r="L44" t="s">
+        <v>247</v>
+      </c>
+      <c r="M44" t="s">
+        <v>236</v>
+      </c>
+      <c r="N44" t="s">
         <v>225</v>
       </c>
-      <c r="L44" t="s">
-        <v>226</v>
-      </c>
-      <c r="M44" t="s">
-        <v>227</v>
-      </c>
-      <c r="N44" t="s">
-        <v>40</v>
+      <c r="Q44" t="s">
+        <v>250</v>
+      </c>
+      <c r="R44" t="s">
+        <v>249</v>
+      </c>
+      <c r="S44" t="s">
+        <v>251</v>
+      </c>
+      <c r="U44" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D45" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E45" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F45" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="G45" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="H45" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="I45" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J45">
-        <v>6700</v>
+        <v>6560</v>
       </c>
       <c r="K45" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="L45" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="M45" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="N45" t="s">
-        <v>40</v>
-      </c>
-      <c r="S45" t="s">
-        <v>74</v>
+        <v>237</v>
+      </c>
+      <c r="O45" t="s">
+        <v>261</v>
+      </c>
+      <c r="R45" t="s">
+        <v>259</v>
+      </c>
+      <c r="T45" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E46" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F46" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="G46" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="H46" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="I46" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J46">
-        <v>6700</v>
+        <v>6560</v>
       </c>
       <c r="K46" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="L46" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="M46" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="N46" t="s">
-        <v>40</v>
-      </c>
-      <c r="S46" t="s">
-        <v>74</v>
+        <v>237</v>
+      </c>
+      <c r="O46" t="s">
+        <v>261</v>
+      </c>
+      <c r="R46" t="s">
+        <v>259</v>
+      </c>
+      <c r="T46" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E47" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F47" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="G47" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="H47" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="I47" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J47">
-        <v>6700</v>
+        <v>6560</v>
       </c>
       <c r="K47" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="L47" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="M47" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="N47" t="s">
-        <v>40</v>
-      </c>
-      <c r="S47" t="s">
-        <v>74</v>
+        <v>237</v>
+      </c>
+      <c r="O47" t="s">
+        <v>261</v>
+      </c>
+      <c r="R47" t="s">
+        <v>259</v>
+      </c>
+      <c r="T47" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="E48" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F48" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="G48" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="H48" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="I48" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="J48">
-        <v>6700</v>
+        <v>6560</v>
       </c>
       <c r="K48" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="L48" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="M48" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="N48" t="s">
-        <v>40</v>
-      </c>
-      <c r="S48" t="s">
-        <v>74</v>
+        <v>237</v>
+      </c>
+      <c r="O48" t="s">
+        <v>261</v>
+      </c>
+      <c r="R48" t="s">
+        <v>259</v>
+      </c>
+      <c r="T48" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>